<commit_message>
Checking in Updated Scripts
</commit_message>
<xml_diff>
--- a/utilities/Excel_Sheets/Products/CRYO.xlsx
+++ b/utilities/Excel_Sheets/Products/CRYO.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="61">
   <si>
     <t>Test_Scenario</t>
   </si>
@@ -204,6 +204,15 @@
   </si>
   <si>
     <t>Revenue (This Year)</t>
+  </si>
+  <si>
+    <t>Los_Angeles_County_California</t>
+  </si>
+  <si>
+    <t>Random City</t>
+  </si>
+  <si>
+    <t>Illinois</t>
   </si>
 </sst>
 </file>
@@ -608,7 +617,7 @@
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -679,7 +688,7 @@
       </c>
       <c r="C2" s="6">
         <f ca="1">TODAY()</f>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>3</v>
@@ -722,7 +731,7 @@
       </c>
       <c r="C4" s="6">
         <f ca="1">TODAY()</f>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>3</v>
@@ -779,7 +788,7 @@
       </c>
       <c r="C6" s="6">
         <f ca="1">TODAY()</f>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>3</v>
@@ -836,7 +845,7 @@
       </c>
       <c r="C8" s="6">
         <f ca="1">TODAY()</f>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>3</v>
@@ -879,7 +888,7 @@
       </c>
       <c r="C10" s="6">
         <f ca="1">TODAY()</f>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>3</v>
@@ -936,7 +945,7 @@
       </c>
       <c r="C12" s="6">
         <f ca="1">TODAY()</f>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>3</v>
@@ -993,7 +1002,7 @@
       </c>
       <c r="C14" s="6">
         <f ca="1">TODAY()</f>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>3</v>
@@ -1038,7 +1047,7 @@
       </c>
       <c r="C16" s="6">
         <f ca="1">TODAY()</f>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>3</v>
@@ -1095,7 +1104,7 @@
       </c>
       <c r="C18" s="6">
         <f ca="1">TODAY()</f>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>3</v>
@@ -1152,7 +1161,7 @@
       </c>
       <c r="C20" s="6">
         <f ca="1">TODAY()</f>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>3</v>
@@ -1209,7 +1218,7 @@
       </c>
       <c r="C22" s="6">
         <f ca="1">TODAY()</f>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>3</v>
@@ -1254,7 +1263,7 @@
       </c>
       <c r="C24" s="6">
         <f ca="1">TODAY()</f>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>3</v>
@@ -1299,7 +1308,7 @@
       </c>
       <c r="C26" s="6">
         <f ca="1">TODAY()</f>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>3</v>
@@ -1356,7 +1365,7 @@
       </c>
       <c r="C28" s="6">
         <f ca="1">TODAY()</f>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>3</v>
@@ -1413,7 +1422,7 @@
       </c>
       <c r="C30" s="6">
         <f ca="1">TODAY()</f>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>3</v>
@@ -1470,7 +1479,7 @@
       </c>
       <c r="C32" s="6">
         <f ca="1">TODAY()</f>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>3</v>
@@ -1527,7 +1536,7 @@
       </c>
       <c r="C34" s="6">
         <f ca="1">TODAY()</f>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>3</v>
@@ -1584,7 +1593,7 @@
       </c>
       <c r="C36" s="6">
         <f ca="1">TODAY()</f>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>3</v>
@@ -1629,7 +1638,7 @@
       </c>
       <c r="C38" s="6">
         <f ca="1">TODAY()</f>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>3</v>
@@ -1674,7 +1683,7 @@
       </c>
       <c r="C40" s="6">
         <f ca="1">TODAY()</f>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>3</v>
@@ -1719,7 +1728,7 @@
       </c>
       <c r="C42" s="6">
         <f ca="1">TODAY()</f>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>3</v>
@@ -1776,7 +1785,7 @@
       </c>
       <c r="C44" s="6">
         <f ca="1">TODAY()</f>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>3</v>
@@ -1833,7 +1842,7 @@
       </c>
       <c r="C46" s="6">
         <f ca="1">TODAY()</f>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>3</v>
@@ -1890,7 +1899,7 @@
       </c>
       <c r="C48" s="6">
         <f ca="1">TODAY()</f>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>3</v>
@@ -1947,7 +1956,7 @@
       </c>
       <c r="C50" s="6">
         <f ca="1">TODAY()</f>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>3</v>
@@ -2004,7 +2013,7 @@
       </c>
       <c r="C52" s="6">
         <f ca="1">TODAY()</f>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>3</v>
@@ -2061,7 +2070,7 @@
       </c>
       <c r="C54" s="6">
         <f ca="1">TODAY()</f>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>3</v>
@@ -2106,7 +2115,7 @@
       </c>
       <c r="C56" s="6">
         <f ca="1">TODAY()</f>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>3</v>
@@ -2163,7 +2172,7 @@
       </c>
       <c r="C58" s="6">
         <f ca="1">TODAY()</f>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>3</v>
@@ -2208,7 +2217,7 @@
       </c>
       <c r="C60" s="6">
         <f ca="1">TODAY()</f>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>3</v>
@@ -2417,10 +2426,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22644E77-FC0A-47A4-9DB5-3D708939BD8E}">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2484,26 +2493,26 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
       </c>
       <c r="C2" s="6">
         <f ca="1">TODAY()</f>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="G2" s="3">
-        <v>91436</v>
+        <v>60601</v>
       </c>
       <c r="H2" s="5">
         <v>1000000</v>
@@ -2515,7 +2524,7 @@
         <v>5</v>
       </c>
       <c r="K2" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L2" s="4">
         <v>0</v>
@@ -2534,7 +2543,7 @@
       </c>
       <c r="C4" s="6">
         <f t="shared" ref="C4:C32" ca="1" si="0">TODAY()</f>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>3</v>
@@ -2576,7 +2585,7 @@
       </c>
       <c r="C5" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>3</v>
@@ -2618,7 +2627,7 @@
       </c>
       <c r="C6" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>3</v>
@@ -2660,7 +2669,7 @@
       </c>
       <c r="C7" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>3</v>
@@ -2702,7 +2711,7 @@
       </c>
       <c r="C8" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>3</v>
@@ -2744,7 +2753,7 @@
       </c>
       <c r="C9" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>3</v>
@@ -2786,7 +2795,7 @@
       </c>
       <c r="C10" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>3</v>
@@ -2828,7 +2837,7 @@
       </c>
       <c r="C11" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>3</v>
@@ -2870,7 +2879,7 @@
       </c>
       <c r="C12" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>3</v>
@@ -2912,7 +2921,7 @@
       </c>
       <c r="C13" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>3</v>
@@ -2954,7 +2963,7 @@
       </c>
       <c r="C14" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>3</v>
@@ -2996,7 +3005,7 @@
       </c>
       <c r="C15" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>3</v>
@@ -3038,7 +3047,7 @@
       </c>
       <c r="C16" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>3</v>
@@ -3080,7 +3089,7 @@
       </c>
       <c r="C17" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>3</v>
@@ -3122,7 +3131,7 @@
       </c>
       <c r="C18" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>3</v>
@@ -3164,7 +3173,7 @@
       </c>
       <c r="C19" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>3</v>
@@ -3206,7 +3215,7 @@
       </c>
       <c r="C20" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>3</v>
@@ -3248,7 +3257,7 @@
       </c>
       <c r="C21" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>3</v>
@@ -3290,7 +3299,7 @@
       </c>
       <c r="C22" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>3</v>
@@ -3332,7 +3341,7 @@
       </c>
       <c r="C23" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>3</v>
@@ -3374,7 +3383,7 @@
       </c>
       <c r="C24" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>3</v>
@@ -3416,7 +3425,7 @@
       </c>
       <c r="C25" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>3</v>
@@ -3458,7 +3467,7 @@
       </c>
       <c r="C26" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>3</v>
@@ -3500,7 +3509,7 @@
       </c>
       <c r="C27" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>3</v>
@@ -3542,7 +3551,7 @@
       </c>
       <c r="C28" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>3</v>
@@ -3584,7 +3593,7 @@
       </c>
       <c r="C29" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>3</v>
@@ -3626,7 +3635,7 @@
       </c>
       <c r="C30" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>3</v>
@@ -3668,7 +3677,7 @@
       </c>
       <c r="C31" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>3</v>
@@ -3710,7 +3719,7 @@
       </c>
       <c r="C32" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43301</v>
+        <v>43308</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>3</v>

</xml_diff>